<commit_message>
entrega experiencia 2 terminado
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javit\Desktop\Exp2_Baeza_Rodriguez_004D\Exp2_Baeza_Rodriguez_004D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866C1F63-E429-4969-89CB-154810288653}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F5A72D-8D04-4C83-A9E1-8DED85C47FA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
@@ -57,46 +57,46 @@
     <t>Alexis Rodriguez y Francisco Baeza</t>
   </si>
   <si>
-    <t xml:space="preserve">Alexis Rodriguez </t>
-  </si>
-  <si>
     <t>Francisco Baeza y Alexis Rodriguez</t>
   </si>
   <si>
     <t xml:space="preserve">Francisco Baeza </t>
   </si>
   <si>
-    <t>Creacion del nombre de la pagina y el logo</t>
-  </si>
-  <si>
-    <t>Iniciamos la contruccion de la pagina index.html</t>
-  </si>
-  <si>
-    <t>Nos reunimos para compartir los bocetos hechos a mano</t>
-  </si>
-  <si>
-    <t>Hicimos bocetos de la pagina web</t>
-  </si>
-  <si>
-    <t>Creacion de la barra navegadora</t>
-  </si>
-  <si>
     <t>Alexis Rodriguez</t>
   </si>
   <si>
-    <t>Nos reunimos via discord para recopilar información</t>
-  </si>
-  <si>
     <t>Redaccion de la bitacora</t>
   </si>
   <si>
-    <t>Creacion pagina "Sobre Nosotros"</t>
-  </si>
-  <si>
-    <t>Creacion pagina "Galeria"</t>
-  </si>
-  <si>
-    <t>Solucion probolemas carrusel con barra navegadora</t>
+    <t>Francisco Baeza</t>
+  </si>
+  <si>
+    <t>Decidimos datos a pedir en los formularios</t>
+  </si>
+  <si>
+    <t>Nos reunimos via discord para ver errores de la entrega anterior</t>
+  </si>
+  <si>
+    <t>Iniciamos la contruccion de los formularios</t>
+  </si>
+  <si>
+    <t>Cambio barra navegadora</t>
+  </si>
+  <si>
+    <t>Busqueda de la API</t>
+  </si>
+  <si>
+    <t>creacion de pagina registro</t>
+  </si>
+  <si>
+    <t>creacion de pagina publicar</t>
+  </si>
+  <si>
+    <t>busquedad de eventos para mouse y pagina oscura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar paginas donde haya referencias para la pagina </t>
   </si>
 </sst>
 </file>
@@ -465,13 +465,13 @@
   <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -497,7 +497,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -516,10 +516,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -538,10 +538,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -549,10 +549,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -560,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -571,10 +571,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -593,10 +593,10 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -604,10 +604,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>

</xml_diff>